<commit_message>
T1: Added Not fully calculed niepewnosc objetosci
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/Cw100_Kulki_Tuleje_Gestosc.xlsx
+++ b/Fizyka_Sprawka/Cw100_Kulki_Tuleje_Gestosc.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="a)-Niepewnosc pomiarowa masy" sheetId="1" r:id="rId1"/>
     <sheet name="b)-Srednica i jej niepewnosc" sheetId="2" r:id="rId2"/>
     <sheet name="c1)V i jej niepewnosc(kula)" sheetId="3" r:id="rId3"/>
+    <sheet name="c1)V i niepewnosc-tuleja" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Kulka</t>
   </si>
@@ -191,6 +192,15 @@
   </si>
   <si>
     <t>Całkowita Niep. Stand.- Obliczenie - Wew</t>
+  </si>
+  <si>
+    <t>15.858 - 12.215</t>
+  </si>
+  <si>
+    <t>3.643^2</t>
+  </si>
+  <si>
+    <t>34.17 * 13.271449</t>
   </si>
 </sst>
 </file>
@@ -759,15 +769,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -775,12 +776,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -807,6 +802,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -825,6 +823,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,13 +847,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -855,16 +871,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -9952,8 +9962,8 @@
       <xdr:rowOff>17367</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2442882" cy="778250"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="50" name="TextBox 49"/>
@@ -10534,7 +10544,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="50" name="TextBox 49"/>
@@ -15651,8 +15661,8 @@
       <xdr:rowOff>9217</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1398524" cy="179665"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="TextBox 37"/>
@@ -15897,7 +15907,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="TextBox 37"/>
@@ -16082,8 +16092,8 @@
       <xdr:rowOff>194896</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1129604" cy="179665"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -16178,7 +16188,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -16190,7 +16200,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -16204,7 +16214,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16217,7 +16227,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16231,7 +16241,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16247,7 +16257,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16260,7 +16270,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16275,7 +16285,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -16288,7 +16298,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -16302,7 +16312,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16316,7 +16326,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -16330,7 +16340,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -16342,7 +16352,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -16354,7 +16364,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -16370,7 +16380,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -16574,8 +16584,8 @@
       <xdr:rowOff>55978</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2433900" cy="689458"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="31" name="TextBox 30"/>
@@ -16982,14 +16992,7 @@
                               <m:nor/>
                             </m:rPr>
                             <a:rPr lang="en-US"/>
-                            <m:t> </m:t>
-                          </m:r>
-                          <m:r>
-                            <m:rPr>
-                              <m:nor/>
-                            </m:rPr>
-                            <a:rPr lang="en-US"/>
-                            <m:t>  </m:t>
+                            <m:t>   </m:t>
                           </m:r>
                           <m:r>
                             <m:rPr>
@@ -17052,11 +17055,7 @@
               </a:r>
               <a:r>
                 <a:rPr lang="en-US"/>
-                <a:t> </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US"/>
-                <a:t> </a:t>
+                <a:t>  </a:t>
               </a:r>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
@@ -17088,7 +17087,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="31" name="TextBox 30"/>
@@ -17495,8 +17494,8 @@
       <xdr:rowOff>10717</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2575472" cy="1076254"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="37" name="TextBox 36"/>
@@ -18204,7 +18203,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="37" name="TextBox 36"/>
@@ -18505,8 +18504,8 @@
       <xdr:rowOff>17367</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2442882" cy="778250"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="40" name="TextBox 39"/>
@@ -18942,14 +18941,7 @@
                           <m:nor/>
                         </m:rPr>
                         <a:rPr lang="en-US"/>
-                        <m:t> </m:t>
-                      </m:r>
-                      <m:r>
-                        <m:rPr>
-                          <m:nor/>
-                        </m:rPr>
-                        <a:rPr lang="en-US"/>
-                        <m:t>  </m:t>
+                        <m:t>   </m:t>
                       </m:r>
                       <m:r>
                         <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
@@ -19036,14 +19028,7 @@
                           <m:nor/>
                         </m:rPr>
                         <a:rPr lang="en-US"/>
-                        <m:t> </m:t>
-                      </m:r>
-                      <m:r>
-                        <m:rPr>
-                          <m:nor/>
-                        </m:rPr>
-                        <a:rPr lang="en-US"/>
-                        <m:t>   </m:t>
+                        <m:t>    </m:t>
                       </m:r>
                     </m:e>
                   </m:rad>
@@ -19079,14 +19064,7 @@
                       <m:nor/>
                     </m:rPr>
                     <a:rPr lang="en-US"/>
-                    <m:t> </m:t>
-                  </m:r>
-                  <m:r>
-                    <m:rPr>
-                      <m:nor/>
-                    </m:rPr>
-                    <a:rPr lang="en-US"/>
-                    <m:t>  </m:t>
+                    <m:t>   </m:t>
                   </m:r>
                 </m:oMath>
               </a14:m>
@@ -19125,7 +19103,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="40" name="TextBox 39"/>
@@ -24867,6 +24845,1780 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>102291</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>23192</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4071499" cy="351828"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1073841" y="2337767"/>
+              <a:ext cx="4071499" cy="351828"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑉</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>=</m:t>
+                  </m:r>
+                  <m:acc>
+                    <m:accPr>
+                      <m:chr m:val="̅"/>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:accPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>h</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:acc>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                  <m:sSup>
+                    <m:sSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑟</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>2</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSup>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>=</m:t>
+                  </m:r>
+                  <m:acc>
+                    <m:accPr>
+                      <m:chr m:val="̅"/>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:accPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>h</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:acc>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                  <m:sSup>
+                    <m:sSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>(</m:t>
+                      </m:r>
+                      <m:acc>
+                        <m:accPr>
+                          <m:chr m:val="̅"/>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1100" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:accPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝑑𝑧𝑒𝑤</m:t>
+                          </m:r>
+                        </m:e>
+                      </m:acc>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US">
+                          <a:effectLst/>
+                        </a:rPr>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="pl-PL" b="0" i="1">
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>−</m:t>
+                      </m:r>
+                      <m:acc>
+                        <m:accPr>
+                          <m:chr m:val="̅"/>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1100" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:accPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝑑𝑤𝑒𝑤</m:t>
+                          </m:r>
+                        </m:e>
+                      </m:acc>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US">
+                          <a:effectLst/>
+                        </a:rPr>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>)</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>2</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSup>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>=</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>34.17∗</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                  <m:sSup>
+                    <m:sSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>(</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>15.858</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>−</m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>12.215</m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>)</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>2</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSup>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100"/>
+                <a:t>=</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>34.17∗</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                  <m:sSup>
+                    <m:sSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>(</m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>3.643</m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US"/>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>)</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>2</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSup>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100"/>
+                <a:t>=</a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>34.17∗</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>*</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>13.271449</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>= 453.4854123</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US"/>
+                <a:t> </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1073841" y="2337767"/>
+              <a:ext cx="4071499" cy="351828"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉=ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋𝑟^2=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜋〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑑𝑧𝑒𝑤</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" b="0" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" −</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑑𝑤𝑒𝑤</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" )</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〗^2=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>34.17∗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜋〖(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>15.858</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>−"12.215</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" )〗^2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100"/>
+                <a:t>=</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>34.17∗𝜋〖(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"3.643</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" )〗^2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100"/>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>34.17∗𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>*</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>13.271449</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>= 453.4854123</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>5442</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="312842" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="65314" y="386442"/>
+              <a:ext cx="312842" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑢</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="65314" y="386442"/>
+              <a:ext cx="312842" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑢(𝑥)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="842015" cy="160852"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="57150" y="790575"/>
+              <a:ext cx="842015" cy="160852"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>h</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="57150" y="790575"/>
+              <a:ext cx="842015" cy="160852"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>50132</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20053</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="842015" cy="160852"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="50132" y="982078"/>
+              <a:ext cx="842015" cy="160852"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑𝑤𝑒𝑤</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="50132" y="982078"/>
+              <a:ext cx="842015" cy="160852"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑𝑤𝑒𝑤</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="842015" cy="160852"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1162050"/>
+              <a:ext cx="842015" cy="160852"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑𝑧𝑒𝑤</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1162050"/>
+              <a:ext cx="842015" cy="160852"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑𝑧𝑒𝑤</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -25151,39 +26903,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="76" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -25192,16 +26944,16 @@
       <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -25211,14 +26963,14 @@
       <c r="B4" s="21">
         <v>0.72</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="69"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="79"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
@@ -25227,40 +26979,40 @@
       <c r="B5" s="22">
         <v>8.24</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="60"/>
-      <c r="H5" s="61"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="78"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="23"/>
-      <c r="C6" s="72">
+      <c r="C6" s="67">
         <v>0.01</v>
       </c>
-      <c r="D6" s="73"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="75"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -25281,12 +27033,12 @@
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -25295,18 +27047,18 @@
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="78"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -25327,12 +27079,12 @@
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="64"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="61"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -25353,18 +27105,18 @@
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
-      <c r="B22" s="66"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="8"/>
       <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="64"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="61"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -25385,12 +27137,12 @@
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="64"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="61"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
@@ -25412,6 +27164,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="J1:Q1"/>
@@ -25427,11 +27184,6 @@
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25443,8 +27195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25468,16 +27220,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="62" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="61"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -25867,86 +27619,86 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="64"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="61"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="62" t="s">
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="64"/>
+      <c r="F16" s="61"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="85" t="s">
+      <c r="A17" s="89"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="79"/>
+      <c r="F17" s="75"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="59" t="s">
+      <c r="A18" s="79"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="61"/>
+      <c r="F18" s="78"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="59" t="s">
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="61"/>
+      <c r="F19" s="78"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="86" t="s">
+      <c r="A20" s="80"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="87"/>
+      <c r="F20" s="94"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="76" t="s">
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="76"/>
-      <c r="K21" s="76" t="s">
+      <c r="H21" s="72"/>
+      <c r="K21" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="L21" s="76"/>
+      <c r="L21" s="72"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -25955,10 +27707,10 @@
       <c r="B22" s="18"/>
       <c r="C22" s="54"/>
       <c r="D22" s="55"/>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="76"/>
+      <c r="F22" s="72"/>
       <c r="G22" s="81" t="s">
         <v>27</v>
       </c>
@@ -25969,14 +27721,14 @@
       <c r="L22" s="82"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="62" t="s">
+      <c r="B23" s="61"/>
+      <c r="C23" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="64"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="27" t="s">
         <v>5</v>
       </c>
@@ -26003,12 +27755,12 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="85"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="85">
+      <c r="A24" s="89"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="89">
         <v>0.05</v>
       </c>
-      <c r="D24" s="79"/>
+      <c r="D24" s="75"/>
       <c r="E24" s="11"/>
       <c r="F24" s="5">
         <v>0.05</v>
@@ -26019,12 +27771,12 @@
       <c r="L24" s="40"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="59"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="59">
+      <c r="A25" s="79"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="79">
         <v>8.1669999999999998</v>
       </c>
-      <c r="D25" s="61"/>
+      <c r="D25" s="78"/>
       <c r="E25" s="81" t="s">
         <v>27</v>
       </c>
@@ -26035,14 +27787,14 @@
       <c r="L25" s="40"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="65">
+      <c r="B26" s="71"/>
+      <c r="C26" s="80">
         <v>10</v>
       </c>
-      <c r="D26" s="75"/>
+      <c r="D26" s="71"/>
       <c r="E26" s="39"/>
       <c r="F26" s="40"/>
       <c r="G26" s="30"/>
@@ -26056,7 +27808,7 @@
       </c>
       <c r="B27" s="82"/>
       <c r="C27" s="82"/>
-      <c r="D27" s="94"/>
+      <c r="D27" s="88"/>
       <c r="E27" s="39"/>
       <c r="F27" s="40"/>
       <c r="G27" s="31" t="s">
@@ -26119,12 +27871,12 @@
       <c r="L31" s="49"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="93"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
       <c r="E32" s="48"/>
       <c r="F32" s="49"/>
       <c r="G32" s="42"/>
@@ -26295,6 +28047,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A16:D16"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="K34:L34"/>
@@ -26309,26 +28079,8 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A16:D16"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26340,8 +28092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H23:H24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="A10:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26585,4 +28337,125 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>34.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6">
+        <v>12.215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7">
+        <v>15.858000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <f>15.858-12.215</f>
+        <v>3.6430000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <f>3.643^2</f>
+        <v>13.271448999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <f>34.17 * 13.271449</f>
+        <v>453.48541233000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B12:D12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>